<commit_message>
Menghapus file tidak terpakai
</commit_message>
<xml_diff>
--- a/absensi.xlsx
+++ b/absensi.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
-  <si>
-    <t>Email address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t>Absensi</t>
   </si>
@@ -37,93 +34,6 @@
   </si>
   <si>
     <t>Penugasan</t>
-  </si>
-  <si>
-    <t>20180910035@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910009@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910008@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910037@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910025@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910016@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910018@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910036@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910027@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910013@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910005@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910026@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910012@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910007@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910031@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180920161@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910011@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910032@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910004@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910017@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910021@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910002@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910001@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910034@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910010@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910003@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910020@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910015@uniku.ac.id</t>
-  </si>
-  <si>
-    <t>20180910033@uniku.ac.id</t>
   </si>
   <si>
     <t>Abdul Latif</t>
@@ -651,529 +561,438 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:E30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>